<commit_message>
Buổi 13: ant design - add product form
</commit_message>
<xml_diff>
--- a/diem_danh_giay_24_03_23_05_55_06.xlsx
+++ b/diem_danh_giay_24_03_23_05_55_06.xlsx
@@ -420,9 +420,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="24">
@@ -467,6 +467,22 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -475,24 +491,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -514,81 +522,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -603,6 +537,72 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -613,25 +613,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -649,7 +631,139 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -661,73 +775,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -739,61 +793,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -831,6 +831,17 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -846,15 +857,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -866,26 +868,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -919,121 +901,139 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="10" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="29" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1045,22 +1045,22 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1482,8 +1482,8 @@
   <sheetPr/>
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="E44" sqref="E44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
@@ -1660,7 +1660,9 @@
       <c r="D6" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="1"/>
+      <c r="E6" s="1">
+        <v>9</v>
+      </c>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
@@ -1696,7 +1698,9 @@
       <c r="D7" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="1"/>
+      <c r="E7" s="1">
+        <v>9</v>
+      </c>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
@@ -1732,7 +1736,9 @@
       <c r="D8" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="E8" s="1"/>
+      <c r="E8" s="1">
+        <v>9</v>
+      </c>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
@@ -1768,7 +1774,9 @@
       <c r="D9" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="E9" s="1"/>
+      <c r="E9" s="1">
+        <v>9</v>
+      </c>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
@@ -1804,7 +1812,9 @@
       <c r="D10" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="E10" s="1"/>
+      <c r="E10" s="1">
+        <v>9</v>
+      </c>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
@@ -1840,7 +1850,9 @@
       <c r="D11" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="E11" s="1"/>
+      <c r="E11" s="1">
+        <v>4</v>
+      </c>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
@@ -1876,7 +1888,9 @@
       <c r="D12" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="E12" s="1"/>
+      <c r="E12" s="1">
+        <v>9</v>
+      </c>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
@@ -1912,7 +1926,9 @@
       <c r="D13" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="E13" s="1"/>
+      <c r="E13" s="1">
+        <v>9</v>
+      </c>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
@@ -1948,7 +1964,9 @@
       <c r="D14" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="E14" s="1"/>
+      <c r="E14" s="1">
+        <v>9</v>
+      </c>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
@@ -1984,7 +2002,9 @@
       <c r="D15" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="E15" s="1"/>
+      <c r="E15" s="1">
+        <v>9</v>
+      </c>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
@@ -2020,7 +2040,9 @@
       <c r="D16" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="E16" s="1"/>
+      <c r="E16" s="1">
+        <v>9</v>
+      </c>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
@@ -2094,7 +2116,9 @@
       <c r="D18" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="E18" s="1"/>
+      <c r="E18" s="1">
+        <v>9</v>
+      </c>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
@@ -2130,7 +2154,9 @@
       <c r="D19" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="E19" s="1"/>
+      <c r="E19" s="1">
+        <v>9</v>
+      </c>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
@@ -2166,7 +2192,9 @@
       <c r="D20" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="E20" s="1"/>
+      <c r="E20" s="1">
+        <v>9</v>
+      </c>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
@@ -2202,7 +2230,9 @@
       <c r="D21" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="E21" s="1"/>
+      <c r="E21" s="1">
+        <v>9</v>
+      </c>
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
@@ -2238,7 +2268,9 @@
       <c r="D22" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="E22" s="1"/>
+      <c r="E22" s="1">
+        <v>9</v>
+      </c>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
@@ -2274,7 +2306,9 @@
       <c r="D23" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="E23" s="1"/>
+      <c r="E23" s="1">
+        <v>4</v>
+      </c>
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
@@ -2310,7 +2344,9 @@
       <c r="D24" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="E24" s="1"/>
+      <c r="E24" s="1">
+        <v>9</v>
+      </c>
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
@@ -2346,7 +2382,9 @@
       <c r="D25" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="E25" s="1"/>
+      <c r="E25" s="1">
+        <v>9</v>
+      </c>
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
@@ -2382,7 +2420,9 @@
       <c r="D26" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="E26" s="1"/>
+      <c r="E26" s="1">
+        <v>9</v>
+      </c>
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
@@ -2418,7 +2458,9 @@
       <c r="D27" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="E27" s="1"/>
+      <c r="E27" s="1">
+        <v>9</v>
+      </c>
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
@@ -2454,7 +2496,9 @@
       <c r="D28" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="E28" s="1"/>
+      <c r="E28" s="1">
+        <v>9</v>
+      </c>
       <c r="F28" s="1"/>
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
@@ -2490,7 +2534,9 @@
       <c r="D29" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="E29" s="1"/>
+      <c r="E29" s="1">
+        <v>9</v>
+      </c>
       <c r="F29" s="1"/>
       <c r="G29" s="1"/>
       <c r="H29" s="1"/>
@@ -2526,7 +2572,9 @@
       <c r="D30" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="E30" s="1"/>
+      <c r="E30" s="1">
+        <v>9</v>
+      </c>
       <c r="F30" s="1"/>
       <c r="G30" s="1"/>
       <c r="H30" s="1"/>
@@ -2562,7 +2610,9 @@
       <c r="D31" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="E31" s="1"/>
+      <c r="E31" s="1">
+        <v>9</v>
+      </c>
       <c r="F31" s="1"/>
       <c r="G31" s="1"/>
       <c r="H31" s="1"/>
@@ -2598,7 +2648,9 @@
       <c r="D32" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="E32" s="1"/>
+      <c r="E32" s="1">
+        <v>9</v>
+      </c>
       <c r="F32" s="1"/>
       <c r="G32" s="1"/>
       <c r="H32" s="1"/>
@@ -2634,7 +2686,9 @@
       <c r="D33" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="E33" s="1"/>
+      <c r="E33" s="1">
+        <v>9</v>
+      </c>
       <c r="F33" s="1"/>
       <c r="G33" s="1"/>
       <c r="H33" s="1"/>
@@ -2670,7 +2724,9 @@
       <c r="D34" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="E34" s="1"/>
+      <c r="E34" s="1">
+        <v>9</v>
+      </c>
       <c r="F34" s="1"/>
       <c r="G34" s="1"/>
       <c r="H34" s="1"/>
@@ -2706,7 +2762,9 @@
       <c r="D35" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="E35" s="1"/>
+      <c r="E35" s="1">
+        <v>9</v>
+      </c>
       <c r="F35" s="1"/>
       <c r="G35" s="1"/>
       <c r="H35" s="1"/>
@@ -2742,7 +2800,9 @@
       <c r="D36" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="E36" s="1"/>
+      <c r="E36" s="1">
+        <v>9</v>
+      </c>
       <c r="F36" s="1"/>
       <c r="G36" s="1"/>
       <c r="H36" s="1"/>
@@ -2778,7 +2838,9 @@
       <c r="D37" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="E37" s="1"/>
+      <c r="E37" s="1">
+        <v>9</v>
+      </c>
       <c r="F37" s="1"/>
       <c r="G37" s="1"/>
       <c r="H37" s="1"/>
@@ -2814,7 +2876,9 @@
       <c r="D38" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="E38" s="1"/>
+      <c r="E38" s="1">
+        <v>9</v>
+      </c>
       <c r="F38" s="1"/>
       <c r="G38" s="1"/>
       <c r="H38" s="1"/>
@@ -2850,7 +2914,9 @@
       <c r="D39" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="E39" s="1"/>
+      <c r="E39" s="1">
+        <v>9</v>
+      </c>
       <c r="F39" s="1"/>
       <c r="G39" s="1"/>
       <c r="H39" s="1"/>
@@ -2886,7 +2952,9 @@
       <c r="D40" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="E40" s="1"/>
+      <c r="E40" s="1">
+        <v>9</v>
+      </c>
       <c r="F40" s="1"/>
       <c r="G40" s="1"/>
       <c r="H40" s="1"/>
@@ -2922,7 +2990,9 @@
       <c r="D41" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="E41" s="1"/>
+      <c r="E41" s="1">
+        <v>9</v>
+      </c>
       <c r="F41" s="1"/>
       <c r="G41" s="1"/>
       <c r="H41" s="1"/>
@@ -2996,7 +3066,9 @@
       <c r="D43" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="E43" s="1"/>
+      <c r="E43" s="1">
+        <v>9</v>
+      </c>
       <c r="F43" s="1"/>
       <c r="G43" s="1"/>
       <c r="H43" s="1"/>
@@ -3032,7 +3104,9 @@
       <c r="D44" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="E44" s="1"/>
+      <c r="E44" s="1">
+        <v>0</v>
+      </c>
       <c r="F44" s="1"/>
       <c r="G44" s="1"/>
       <c r="H44" s="1"/>

</xml_diff>